<commit_message>
Refactored existing test cases & property file read utility
</commit_message>
<xml_diff>
--- a/HybridFrameworkOpenCartAutomation/src/test/resources/testData.xlsx
+++ b/HybridFrameworkOpenCartAutomation/src/test/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>UserName</t>
   </si>
@@ -103,6 +103,27 @@
   </si>
   <si>
     <t>Sort by popularity</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Gaoan Bhag</t>
+  </si>
+  <si>
+    <t>Kolhapur</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -584,31 +605,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>